<commit_message>
modity in 0419 night
</commit_message>
<xml_diff>
--- a/Insure_Product_Comparation.xlsx
+++ b/Insure_Product_Comparation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20415" windowHeight="9345"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20412" windowHeight="9348"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="66">
   <si>
     <t>产品</t>
   </si>
@@ -458,6 +458,62 @@
   </si>
   <si>
     <t>苏黎世</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>长期意外</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>至70岁</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>万</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>万</t>
+    </r>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -665,7 +721,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,6 +813,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -764,69 +826,6 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF4F81BD"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -867,25 +866,14 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -895,6 +883,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -922,7 +917,7 @@
           <bgColor rgb="FF4F81BD"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1145,6 +1140,40 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1166,7 +1195,7 @@
           <bgColor rgb="FF4F81BD"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1225,13 +1254,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1241,6 +1263,13 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1268,7 +1297,7 @@
           <bgColor rgb="FF4F81BD"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1500,6 +1529,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1509,6 +1554,27 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1516,12 +1582,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1529,30 +1591,82 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="8778240"/>
+          <a:ext cx="6858000" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B1:H8" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="30" tableBorderDxfId="31" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B1:H8" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="B1:H8"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="产品" dataDxfId="28"/>
-    <tableColumn id="2" name="保障内容" dataDxfId="27"/>
-    <tableColumn id="3" name="保障期限" dataDxfId="26"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="25"/>
-    <tableColumn id="5" name="保障额度" dataDxfId="24"/>
-    <tableColumn id="6" name="保费" dataDxfId="23"/>
-    <tableColumn id="7" name="备注" dataDxfId="22"/>
+    <tableColumn id="1" name="产品" dataDxfId="27"/>
+    <tableColumn id="2" name="保障内容" dataDxfId="26"/>
+    <tableColumn id="3" name="保障期限" dataDxfId="25"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="24"/>
+    <tableColumn id="5" name="保障额度" dataDxfId="23"/>
+    <tableColumn id="6" name="保费" dataDxfId="22"/>
+    <tableColumn id="7" name="备注" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="B10:H19" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="19" tableBorderDxfId="20" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="B10:H19" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B10:H19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="产品"/>
     <tableColumn id="2" name="保障内容"/>
     <tableColumn id="3" name="保障期限"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="17"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="16"/>
     <tableColumn id="5" name="保障额度"/>
     <tableColumn id="6" name="保费"/>
     <tableColumn id="7" name="备注"/>
@@ -1562,29 +1676,29 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="B21:H30" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="B21:H30" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="B21:H30"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="产品" dataDxfId="15"/>
-    <tableColumn id="2" name="保障内容" dataDxfId="14"/>
-    <tableColumn id="3" name="保障期限" dataDxfId="13"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="12"/>
-    <tableColumn id="5" name="保障额度" dataDxfId="11"/>
-    <tableColumn id="6" name="保费" dataDxfId="10"/>
-    <tableColumn id="7" name="备注" dataDxfId="9"/>
+    <tableColumn id="1" name="产品" dataDxfId="11"/>
+    <tableColumn id="2" name="保障内容" dataDxfId="10"/>
+    <tableColumn id="3" name="保障期限" dataDxfId="9"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="8"/>
+    <tableColumn id="5" name="保障额度" dataDxfId="7"/>
+    <tableColumn id="6" name="保费" dataDxfId="6"/>
+    <tableColumn id="7" name="备注" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表2_5" displayName="表2_5" ref="B32:H42" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2" totalsRowBorderDxfId="0">
-  <autoFilter ref="B32:H42"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表2_5" displayName="表2_5" ref="B32:H43" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+  <autoFilter ref="B32:H43"/>
   <tableColumns count="7">
     <tableColumn id="1" name="产品"/>
     <tableColumn id="2" name="保障内容"/>
     <tableColumn id="3" name="保障期限"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="4"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="0"/>
     <tableColumn id="5" name="保障额度"/>
     <tableColumn id="6" name="保费"/>
     <tableColumn id="7" name="备注"/>
@@ -1878,21 +1992,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="10.25" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15">
+    <row r="1" spans="1:8">
       <c r="A1" s="30" t="s">
         <v>56</v>
       </c>
@@ -1918,7 +2034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="28" t="s">
         <v>57</v>
       </c>
@@ -1942,7 +2058,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="14.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
@@ -1968,7 +2084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
@@ -1992,7 +2108,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="14.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
         <v>57</v>
       </c>
@@ -2012,7 +2128,7 @@
       </c>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="14.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="28" t="s">
         <v>57</v>
       </c>
@@ -2036,7 +2152,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8" ht="14.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="28" t="s">
         <v>57</v>
       </c>
@@ -2058,7 +2174,7 @@
       </c>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="14.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="5"/>
       <c r="B8" s="15" t="s">
         <v>28</v>
@@ -2072,7 +2188,7 @@
       </c>
       <c r="H8" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="15">
+    <row r="10" spans="1:8">
       <c r="A10" s="30" t="s">
         <v>56</v>
       </c>
@@ -2098,7 +2214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="28" t="s">
         <v>58</v>
       </c>
@@ -2122,7 +2238,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8" ht="14.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="28" t="s">
         <v>58</v>
       </c>
@@ -2144,7 +2260,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:8" ht="14.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="28" t="s">
         <v>59</v>
       </c>
@@ -2170,7 +2286,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="28" t="s">
         <v>59</v>
       </c>
@@ -2188,7 +2304,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="14.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="28" t="s">
         <v>60</v>
       </c>
@@ -2212,7 +2328,7 @@
       </c>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" ht="14.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="28" t="s">
         <v>60</v>
       </c>
@@ -2230,7 +2346,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8" ht="14.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="28" t="s">
         <v>60</v>
       </c>
@@ -2248,7 +2364,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8" ht="14.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="28" t="s">
         <v>60</v>
       </c>
@@ -2266,7 +2382,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8" ht="14.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="5"/>
       <c r="B19" s="22" t="s">
         <v>28</v>
@@ -2280,7 +2396,7 @@
       </c>
       <c r="H19" s="18"/>
     </row>
-    <row r="21" spans="1:8" ht="15">
+    <row r="21" spans="1:8">
       <c r="A21" s="30" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +2422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="28" t="s">
         <v>57</v>
       </c>
@@ -2330,7 +2446,7 @@
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8" ht="14.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="28" t="s">
         <v>57</v>
       </c>
@@ -2356,7 +2472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="28" t="s">
         <v>57</v>
       </c>
@@ -2380,7 +2496,7 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="14.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="28" t="s">
         <v>57</v>
       </c>
@@ -2400,7 +2516,7 @@
       </c>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8" ht="14.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="28" t="s">
         <v>57</v>
       </c>
@@ -2422,7 +2538,7 @@
       </c>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" ht="14.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="28" t="s">
         <v>57</v>
       </c>
@@ -2446,7 +2562,7 @@
       </c>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8" ht="14.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="28" t="s">
         <v>57</v>
       </c>
@@ -2470,7 +2586,7 @@
       </c>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8" ht="14.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="28" t="s">
         <v>57</v>
       </c>
@@ -2494,7 +2610,7 @@
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8" ht="14.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="5"/>
       <c r="B30" s="15" t="s">
         <v>28</v>
@@ -2509,7 +2625,7 @@
       </c>
       <c r="H30" s="18"/>
     </row>
-    <row r="32" spans="1:8" ht="15">
+    <row r="32" spans="1:8">
       <c r="A32" s="30" t="s">
         <v>56</v>
       </c>
@@ -2535,7 +2651,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="14.25">
+    <row r="33" spans="1:8">
       <c r="A33" s="28" t="s">
         <v>58</v>
       </c>
@@ -2559,7 +2675,7 @@
       </c>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8" ht="14.25">
+    <row r="34" spans="1:8">
       <c r="A34" s="28" t="s">
         <v>58</v>
       </c>
@@ -2581,7 +2697,7 @@
       <c r="G34" s="11"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" ht="14.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="28" t="s">
         <v>57</v>
       </c>
@@ -2598,14 +2714,14 @@
         <v>10</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="G35" s="7">
-        <v>2960</v>
+        <v>3256</v>
       </c>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8" ht="14.25">
+    <row r="36" spans="1:8">
       <c r="A36" s="28" t="s">
         <v>57</v>
       </c>
@@ -2622,16 +2738,16 @@
         <v>10</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G36" s="12">
-        <v>1530</v>
+        <v>1700</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.25">
+    <row r="37" spans="1:8">
       <c r="A37" s="28" t="s">
         <v>57</v>
       </c>
@@ -2647,111 +2763,140 @@
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="12">
-        <v>123.85</v>
+        <v>64.47</v>
       </c>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8" ht="14.25">
+    <row r="38" spans="1:8">
       <c r="A38" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>23</v>
+        <v>57</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="32" t="s">
+        <v>62</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="G38" s="12">
-        <v>892</v>
+        <v>585</v>
       </c>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" ht="14.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="B39" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="1:8" ht="14.25">
+      <c r="E39" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G39" s="12">
+        <v>892</v>
+      </c>
+      <c r="H39" s="14"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="10" t="s">
+      <c r="B40" s="19"/>
+      <c r="C40" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12">
-        <v>100</v>
-      </c>
-      <c r="G40" s="11"/>
-      <c r="H40" s="14"/>
-    </row>
-    <row r="41" spans="1:8" ht="14.25">
+      <c r="E40" s="6"/>
+      <c r="F40" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="5" t="s">
+      <c r="B41" s="20"/>
+      <c r="C41" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12">
+        <v>100</v>
+      </c>
+      <c r="G41" s="11"/>
+      <c r="H41" s="14"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7">
+      <c r="E42" s="6"/>
+      <c r="F42" s="7">
         <v>5000</v>
       </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="1:8" ht="14.25">
-      <c r="A42" s="28"/>
-      <c r="B42" s="22" t="s">
+      <c r="G42" s="6"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="28"/>
+      <c r="B43" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="24">
-        <f>SUM(G33:G41)</f>
-        <v>8770.85</v>
-      </c>
-      <c r="H42" s="18"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="23"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="24">
+        <f>SUM(G33:G42)</f>
+        <v>9762.4699999999993</v>
+      </c>
+      <c r="H43" s="18"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="G45">
+        <v>5600</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
   <tableParts count="4">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2764,7 +2909,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
@@ -2801,7 +2946,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add two docx files
</commit_message>
<xml_diff>
--- a/Insure_Product_Comparation.xlsx
+++ b/Insure_Product_Comparation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20412" windowHeight="9348"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20415" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="68">
   <si>
     <t>产品</t>
   </si>
@@ -514,6 +514,26 @@
       </rPr>
       <t>万</t>
     </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>万</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>附加全残</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -721,7 +741,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -819,13 +839,118 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="37">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFDBE5F1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1591,82 +1716,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>670560</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="8778240"/>
-          <a:ext cx="6858000" cy="1866900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="1">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B1:H8" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="B1:H8" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="B1:H8"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="产品" dataDxfId="27"/>
-    <tableColumn id="2" name="保障内容" dataDxfId="26"/>
-    <tableColumn id="3" name="保障期限" dataDxfId="25"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="24"/>
-    <tableColumn id="5" name="保障额度" dataDxfId="23"/>
-    <tableColumn id="6" name="保费" dataDxfId="22"/>
-    <tableColumn id="7" name="备注" dataDxfId="21"/>
+    <tableColumn id="1" name="产品" dataDxfId="32"/>
+    <tableColumn id="2" name="保障内容" dataDxfId="31"/>
+    <tableColumn id="3" name="保障期限" dataDxfId="30"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="29"/>
+    <tableColumn id="5" name="保障额度" dataDxfId="28"/>
+    <tableColumn id="6" name="保费" dataDxfId="27"/>
+    <tableColumn id="7" name="备注" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="B10:H19" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="B10:H19" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="B10:H19"/>
   <tableColumns count="7">
     <tableColumn id="1" name="产品"/>
     <tableColumn id="2" name="保障内容"/>
     <tableColumn id="3" name="保障期限"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="16"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="21"/>
     <tableColumn id="5" name="保障额度"/>
     <tableColumn id="6" name="保费"/>
     <tableColumn id="7" name="备注"/>
@@ -1676,29 +1749,45 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="B21:H30" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表1_4" displayName="表1_4" ref="B21:H30" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="19" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="B21:H30"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="产品" dataDxfId="11"/>
-    <tableColumn id="2" name="保障内容" dataDxfId="10"/>
-    <tableColumn id="3" name="保障期限" dataDxfId="9"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="8"/>
-    <tableColumn id="5" name="保障额度" dataDxfId="7"/>
-    <tableColumn id="6" name="保费" dataDxfId="6"/>
-    <tableColumn id="7" name="备注" dataDxfId="5"/>
+    <tableColumn id="1" name="产品" dataDxfId="16"/>
+    <tableColumn id="2" name="保障内容" dataDxfId="15"/>
+    <tableColumn id="3" name="保障期限" dataDxfId="14"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="13"/>
+    <tableColumn id="5" name="保障额度" dataDxfId="12"/>
+    <tableColumn id="6" name="保费" dataDxfId="11"/>
+    <tableColumn id="7" name="备注" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表2_5" displayName="表2_5" ref="B32:H43" totalsRowShown="0" headerRowDxfId="4" headerRowBorderDxfId="3" tableBorderDxfId="2" totalsRowBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="表2_5" displayName="表2_5" ref="B32:H43" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B32:H43"/>
   <tableColumns count="7">
     <tableColumn id="1" name="产品"/>
     <tableColumn id="2" name="保障内容"/>
     <tableColumn id="3" name="保障期限"/>
-    <tableColumn id="4" name="缴费期限" dataDxfId="0"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="5"/>
+    <tableColumn id="5" name="保障额度"/>
+    <tableColumn id="6" name="保费"/>
+    <tableColumn id="7" name="备注"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="表2_56" displayName="表2_56" ref="B46:H53" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2" totalsRowBorderDxfId="0">
+  <autoFilter ref="B46:H53"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="产品"/>
+    <tableColumn id="2" name="保障内容"/>
+    <tableColumn id="3" name="保障期限"/>
+    <tableColumn id="4" name="缴费期限" dataDxfId="4"/>
     <tableColumn id="5" name="保障额度"/>
     <tableColumn id="6" name="保费"/>
     <tableColumn id="7" name="备注"/>
@@ -1992,23 +2081,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
-    <col min="4" max="5" width="11.77734375" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="18.375" customWidth="1"/>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="30" t="s">
         <v>56</v>
       </c>
@@ -2034,7 +2123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.25">
       <c r="A2" s="28" t="s">
         <v>57</v>
       </c>
@@ -2058,7 +2147,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="14.25">
       <c r="A3" s="28" t="s">
         <v>57</v>
       </c>
@@ -2084,7 +2173,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="14.25">
       <c r="A4" s="28" t="s">
         <v>57</v>
       </c>
@@ -2108,7 +2197,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="14.25">
       <c r="A5" s="28" t="s">
         <v>57</v>
       </c>
@@ -2128,7 +2217,7 @@
       </c>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="14.25">
       <c r="A6" s="28" t="s">
         <v>57</v>
       </c>
@@ -2152,7 +2241,7 @@
       </c>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="14.25">
       <c r="A7" s="28" t="s">
         <v>57</v>
       </c>
@@ -2174,7 +2263,7 @@
       </c>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="14.25">
       <c r="A8" s="5"/>
       <c r="B8" s="15" t="s">
         <v>28</v>
@@ -2188,7 +2277,7 @@
       </c>
       <c r="H8" s="18"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="30" t="s">
         <v>56</v>
       </c>
@@ -2214,7 +2303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="14.25">
       <c r="A11" s="28" t="s">
         <v>58</v>
       </c>
@@ -2238,7 +2327,7 @@
       </c>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="14.25">
       <c r="A12" s="28" t="s">
         <v>58</v>
       </c>
@@ -2260,7 +2349,7 @@
       <c r="G12" s="11"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="14.25">
       <c r="A13" s="28" t="s">
         <v>59</v>
       </c>
@@ -2286,7 +2375,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="14.25">
       <c r="A14" s="28" t="s">
         <v>59</v>
       </c>
@@ -2304,7 +2393,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="14.25">
       <c r="A15" s="28" t="s">
         <v>60</v>
       </c>
@@ -2328,7 +2417,7 @@
       </c>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="14.25">
       <c r="A16" s="28" t="s">
         <v>60</v>
       </c>
@@ -2346,7 +2435,7 @@
       <c r="G16" s="6"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="14.25">
       <c r="A17" s="28" t="s">
         <v>60</v>
       </c>
@@ -2364,7 +2453,7 @@
       <c r="G17" s="11"/>
       <c r="H17" s="14"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="14.25">
       <c r="A18" s="28" t="s">
         <v>60</v>
       </c>
@@ -2382,7 +2471,7 @@
       <c r="G18" s="6"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="14.25">
       <c r="A19" s="5"/>
       <c r="B19" s="22" t="s">
         <v>28</v>
@@ -2396,7 +2485,7 @@
       </c>
       <c r="H19" s="18"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="30" t="s">
         <v>56</v>
       </c>
@@ -2422,7 +2511,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="14.25">
       <c r="A22" s="28" t="s">
         <v>57</v>
       </c>
@@ -2446,7 +2535,7 @@
       </c>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" ht="14.25">
       <c r="A23" s="28" t="s">
         <v>57</v>
       </c>
@@ -2472,7 +2561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="14.25">
       <c r="A24" s="28" t="s">
         <v>57</v>
       </c>
@@ -2496,7 +2585,7 @@
       </c>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="14.25">
       <c r="A25" s="28" t="s">
         <v>57</v>
       </c>
@@ -2516,7 +2605,7 @@
       </c>
       <c r="H25" s="14"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="14.25">
       <c r="A26" s="28" t="s">
         <v>57</v>
       </c>
@@ -2538,7 +2627,7 @@
       </c>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="14.25">
       <c r="A27" s="28" t="s">
         <v>57</v>
       </c>
@@ -2562,7 +2651,7 @@
       </c>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="14.25">
       <c r="A28" s="28" t="s">
         <v>57</v>
       </c>
@@ -2586,7 +2675,7 @@
       </c>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="14.25">
       <c r="A29" s="28" t="s">
         <v>57</v>
       </c>
@@ -2610,7 +2699,7 @@
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="14.25">
       <c r="A30" s="5"/>
       <c r="B30" s="15" t="s">
         <v>28</v>
@@ -2625,7 +2714,7 @@
       </c>
       <c r="H30" s="18"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="30" t="s">
         <v>56</v>
       </c>
@@ -2651,7 +2740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="14.25">
       <c r="A33" s="28" t="s">
         <v>58</v>
       </c>
@@ -2675,7 +2764,7 @@
       </c>
       <c r="H33" s="8"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="14.25">
       <c r="A34" s="28" t="s">
         <v>58</v>
       </c>
@@ -2697,7 +2786,7 @@
       <c r="G34" s="11"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="14.25">
       <c r="A35" s="28" t="s">
         <v>57</v>
       </c>
@@ -2721,7 +2810,7 @@
       </c>
       <c r="H35" s="8"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="14.25">
       <c r="A36" s="28" t="s">
         <v>57</v>
       </c>
@@ -2747,7 +2836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="14.25">
       <c r="A37" s="28" t="s">
         <v>57</v>
       </c>
@@ -2767,7 +2856,7 @@
       </c>
       <c r="H37" s="14"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" ht="14.25">
       <c r="A38" s="28" t="s">
         <v>57</v>
       </c>
@@ -2789,7 +2878,7 @@
       </c>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" ht="14.25">
       <c r="A39" s="28" t="s">
         <v>60</v>
       </c>
@@ -2813,7 +2902,7 @@
       </c>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" ht="14.25">
       <c r="A40" s="28" t="s">
         <v>60</v>
       </c>
@@ -2831,7 +2920,7 @@
       <c r="G40" s="6"/>
       <c r="H40" s="8"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" ht="14.25">
       <c r="A41" s="28" t="s">
         <v>60</v>
       </c>
@@ -2849,7 +2938,7 @@
       <c r="G41" s="11"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" ht="14.25">
       <c r="A42" s="28" t="s">
         <v>60</v>
       </c>
@@ -2867,7 +2956,7 @@
       <c r="G42" s="6"/>
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" ht="14.25">
       <c r="A43" s="28"/>
       <c r="B43" s="22" t="s">
         <v>28</v>
@@ -2882,17 +2971,179 @@
       </c>
       <c r="H43" s="18"/>
     </row>
-    <row r="45" spans="1:8">
-      <c r="G45">
-        <v>5600</v>
-      </c>
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="14.25">
+      <c r="A47" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" s="7">
+        <v>2305</v>
+      </c>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="1:8" ht="14.25">
+      <c r="A48" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48" s="11"/>
+      <c r="H48" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="14.25">
+      <c r="A49" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G49" s="12">
+        <v>892</v>
+      </c>
+      <c r="H49" s="14"/>
+    </row>
+    <row r="50" spans="1:8" ht="14.25">
+      <c r="A50" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="1:8" ht="14.25">
+      <c r="A51" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12">
+        <v>100</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="14"/>
+    </row>
+    <row r="52" spans="1:8" ht="14.25">
+      <c r="A52" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="19"/>
+      <c r="C52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="6"/>
+      <c r="F52" s="7">
+        <v>5000</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="1:8" ht="14.25">
+      <c r="A53" s="28"/>
+      <c r="B53" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="24">
+        <f>SUM(G47:G52)</f>
+        <v>3197</v>
+      </c>
+      <c r="H53" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="5">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2909,7 +3160,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1">
@@ -2946,7 +3197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add my insurance policy, update xlsx
</commit_message>
<xml_diff>
--- a/Insure_Product_Comparation.xlsx
+++ b/Insure_Product_Comparation.xlsx
@@ -138,8 +138,11 @@
     <t>意外险</t>
   </si>
   <si>
-    <r>
-      <t>100</t>
+    <t>意外医疗</t>
+  </si>
+  <si>
+    <r>
+      <t>5</t>
     </r>
     <r>
       <rPr>
@@ -153,11 +156,74 @@
     </r>
   </si>
   <si>
-    <t>意外医疗</t>
-  </si>
-  <si>
-    <r>
-      <t>5</t>
+    <t>意外津贴险</t>
+  </si>
+  <si>
+    <t>扩展社保用药</t>
+  </si>
+  <si>
+    <t>45+6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>重疾</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>保险公司</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>平安</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国人保</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>苏黎世</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>长期意外</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>至70岁</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>年</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>15</t>
     </r>
     <r>
       <rPr>
@@ -169,76 +235,11 @@
       </rPr>
       <t>万</t>
     </r>
-  </si>
-  <si>
-    <t>意外津贴险</t>
-  </si>
-  <si>
-    <t>扩展社保用药</t>
-  </si>
-  <si>
-    <t>45+6</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>重疾</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>保险公司</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>平安</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>中国人保</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>苏黎世</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>长期意外</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>至70岁</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>30</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>年</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>15</t>
+      <t>16</t>
     </r>
     <r>
       <rPr>
@@ -253,19 +254,7 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>万</t>
-    </r>
+    <t>49万</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -971,7 +960,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -986,7 +975,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1012,7 +1001,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>19</v>
@@ -1036,13 +1025,13 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>10</v>
@@ -1058,7 +1047,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -1073,7 +1062,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G4" s="7">
         <v>2368</v>
@@ -1082,13 +1071,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>9</v>
@@ -1097,7 +1086,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="12">
         <v>1275</v>
@@ -1108,7 +1097,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>13</v>
@@ -1128,20 +1117,20 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="G7" s="12">
         <v>585</v>
@@ -1150,7 +1139,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>22</v>
@@ -1165,56 +1154,56 @@
         <v>17</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="G8" s="12">
-        <v>892</v>
+        <v>641</v>
       </c>
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="16"/>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="11"/>
       <c r="F10" s="12">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>16</v>
@@ -1237,7 +1226,7 @@
       <c r="F12" s="19"/>
       <c r="G12" s="20">
         <f>SUM(G2:G11)</f>
-        <v>8438.64</v>
+        <v>8187.64</v>
       </c>
       <c r="H12" s="15"/>
     </row>

</xml_diff>